<commit_message>
fixed 2 digits in one contour
</commit_message>
<xml_diff>
--- a/Grades_sheet.xlsx
+++ b/Grades_sheet.xlsx
@@ -970,7 +970,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>114128</t>
+          <t>1180128</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -986,7 +986,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>114045</t>
+          <t>1140155</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1060,7 +1060,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>118456</t>
+          <t>1180656</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1088,7 +1088,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>118151</t>
+          <t>1180551</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1100,7 +1100,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>114101</t>
+          <t>1180101</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1116,7 +1116,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>11802045</t>
+          <t>118077045</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1176,7 +1176,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>14111</t>
+          <t>111111</t>
         </is>
       </c>
       <c r="B18" t="n">

</xml_diff>

<commit_message>
fixed the runnig error problem
</commit_message>
<xml_diff>
--- a/Grades_sheet.xlsx
+++ b/Grades_sheet.xlsx
@@ -26,18 +26,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -941,13 +934,12 @@
           <t>1180236</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -957,14 +949,13 @@
           <t>1180333</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>4</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -973,129 +964,134 @@
           <t>1180128</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>5</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1140155</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="inlineStr"/>
-      <c r="D5" t="n">
-        <v>2</v>
+          <t>1180255</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1180114</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
+          <t>1180214</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1180056</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
+          <t>101056</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1140011</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>6</v>
+          <t>1180041</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1180606</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>5</v>
+          <t>101605</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1180656</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+          <t>1180056</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2100011</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>6</v>
+          <t>2200011</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1180551</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+          <t>1180552</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1103,30 +1099,28 @@
           <t>1180101</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>3</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>118077045</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>5</v>
+          <t>1180045</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1135,14 +1129,13 @@
           <t>1180212</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>4</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1151,40 +1144,43 @@
           <t>1180155</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>8</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1170343</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>4</v>
+          <t>11048</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>111111</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="inlineStr"/>
-      <c r="D18" t="n">
-        <v>5</v>
+          <t>1180112</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
best accuracy till now
</commit_message>
<xml_diff>
--- a/Grades_sheet.xlsx
+++ b/Grades_sheet.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -934,14 +941,11 @@
           <t>1180236</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -957,6 +961,7 @@
       <c r="C3" t="n">
         <v>0</v>
       </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -966,12 +971,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -981,42 +985,41 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1180214</t>
+          <t>1180274</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>101056</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+          <t>1180056</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1024,89 +1027,77 @@
           <t>1180041</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>101605</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+          <t>1180606</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1180056</t>
+          <t>1180456</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2200011</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>2200022</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1180552</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+          <t>11180552</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1180101</t>
+          <t>11180207</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1114,14 +1105,9 @@
           <t>1180045</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" s="1" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1131,12 +1117,13 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1146,42 +1133,43 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>11048</t>
+          <t>11170343</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1180112</t>
+          <t>1180172</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed the id a little bit
</commit_message>
<xml_diff>
--- a/Grades_sheet.xlsx
+++ b/Grades_sheet.xlsx
@@ -941,7 +941,11 @@
           <t>1180236</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C2" t="n">
         <v>2</v>
       </c>
@@ -971,7 +975,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
@@ -996,7 +1000,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1180274</t>
+          <t>1180210</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1015,7 +1019,11 @@
           <t>1180056</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="C7" t="n">
         <v>2</v>
       </c>
@@ -1024,10 +1032,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1180041</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>1180001</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="C8" t="n">
         <v>5</v>
       </c>
@@ -1036,10 +1048,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1180606</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
+          <t>1180605</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
       <c r="C9" t="n">
         <v>5</v>
       </c>
@@ -1053,7 +1069,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1067,7 +1083,11 @@
           <t>2200022</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C11" t="n">
         <v>3</v>
       </c>
@@ -1076,10 +1096,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11180552</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+          <t>1180552</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
@@ -1088,12 +1112,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>11180207</t>
+          <t>1180201</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
@@ -1102,10 +1126,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1180045</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>1180015</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
     </row>
@@ -1144,7 +1172,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>11170343</t>
+          <t>111046</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1165,7 +1193,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>

</xml_diff>